<commit_message>
test file 1.xlsx, fixed one error in officer last name, changed the test file to accomodate annonymised test file
</commit_message>
<xml_diff>
--- a/src/main/resources/test file 1.xlsx
+++ b/src/main/resources/test file 1.xlsx
@@ -432,11 +432,11 @@
   </sheetPr>
   <dimension ref="A1:H177"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A154" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C167" activeCellId="0" sqref="C167"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.85"/>
@@ -726,7 +726,7 @@
         <v>25</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C16" s="4" t="n">
         <v>44350.2491898148</v>

</xml_diff>

<commit_message>
Already anonymised, Officer names were simplified in test files
</commit_message>
<xml_diff>
--- a/src/main/resources/test file 1.xlsx
+++ b/src/main/resources/test file 1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="49">
   <si>
     <t xml:space="preserve">Report Title:</t>
   </si>
@@ -76,7 +76,7 @@
     <t xml:space="preserve">Contractor/Vendor Number</t>
   </si>
   <si>
-    <t xml:space="preserve">Officer 1</t>
+    <t xml:space="preserve">Officer</t>
   </si>
   <si>
     <t xml:space="preserve">Contractor </t>
@@ -100,13 +100,7 @@
     <t xml:space="preserve">PLA0102 - Turnstile West IN</t>
   </si>
   <si>
-    <t xml:space="preserve">Officer 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Thames LSI0904 - Turnstile North OUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Officer 3</t>
   </si>
   <si>
     <t xml:space="preserve">Thames LSI0903 - Turnstile North IN</t>
@@ -121,19 +115,7 @@
     <t xml:space="preserve">Thames LSI0902 - Turnstile South OUT</t>
   </si>
   <si>
-    <t xml:space="preserve">Officer 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Officer 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Officer 6</t>
-  </si>
-  <si>
     <t xml:space="preserve">Thames LSI0701 - Weighbridge IN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Officer 7</t>
   </si>
   <si>
     <t xml:space="preserve">Thames LSI1202 - TIE Vehicle IN</t>
@@ -181,22 +163,7 @@
     <t xml:space="preserve">Thames LSI0602 - 1st Floor Central</t>
   </si>
   <si>
-    <t xml:space="preserve">Officer 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Officer 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Officer 10</t>
-  </si>
-  <si>
     <t xml:space="preserve">Thames LSI0702 - Weighbridge OUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Officer 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Officer 12</t>
   </si>
   <si>
     <t xml:space="preserve">Thames LSI0502 - HR Office West</t>
@@ -338,11 +305,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -429,11 +396,11 @@
   </sheetPr>
   <dimension ref="A1:H177"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8:G177"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.85"/>
@@ -514,8 +481,8 @@
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>18</v>
+      <c r="B8" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="C8" s="4" t="n">
         <v>44350.2452314815</v>
@@ -540,8 +507,8 @@
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>18</v>
+      <c r="B9" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="C9" s="4" t="n">
         <v>44350.745162037</v>
@@ -563,22 +530,22 @@
       </c>
     </row>
     <row r="10" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="6" t="n">
+      <c r="A10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5" t="n">
         <v>44350.7459837963</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="6" t="s">
         <v>25</v>
       </c>
       <c r="G10" s="3" t="s">
@@ -592,8 +559,8 @@
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>18</v>
+      <c r="B11" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="C11" s="4" t="n">
         <v>44350.8510532407</v>
@@ -618,8 +585,8 @@
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>18</v>
+      <c r="B12" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="C12" s="4" t="n">
         <v>44350.8643634259</v>
@@ -644,8 +611,8 @@
       <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>18</v>
+      <c r="B13" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="C13" s="4" t="n">
         <v>44351.0835763889</v>
@@ -670,8 +637,8 @@
       <c r="A14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>18</v>
+      <c r="B14" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="C14" s="4" t="n">
         <v>44351.0970949074</v>
@@ -693,22 +660,22 @@
       </c>
     </row>
     <row r="15" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="6" t="n">
+      <c r="A15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5" t="n">
         <v>44351.2466666667</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="6" t="s">
         <v>21</v>
       </c>
       <c r="G15" s="3" t="s">
@@ -720,10 +687,10 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>26</v>
+        <v>18</v>
+      </c>
+      <c r="B16" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="C16" s="4" t="n">
         <v>44350.2491898148</v>
@@ -735,33 +702,33 @@
         <v>20</v>
       </c>
       <c r="F16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="C17" s="5" t="n">
+        <v>44350.2485763889</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="6" t="n">
-        <v>44350.2485763889</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>22</v>
@@ -772,10 +739,10 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
+      </c>
+      <c r="B18" s="3" t="n">
+        <v>3</v>
       </c>
       <c r="C18" s="4" t="n">
         <v>44350.3896412037</v>
@@ -787,7 +754,7 @@
         <v>20</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>22</v>
@@ -798,10 +765,10 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="n">
+        <v>3</v>
       </c>
       <c r="C19" s="4" t="n">
         <v>44350.4067361111</v>
@@ -813,7 +780,7 @@
         <v>20</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>22</v>
@@ -824,10 +791,10 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
+      </c>
+      <c r="B20" s="3" t="n">
+        <v>3</v>
       </c>
       <c r="C20" s="4" t="n">
         <v>44350.407025463</v>
@@ -839,7 +806,7 @@
         <v>20</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>22</v>
@@ -850,10 +817,10 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
+      </c>
+      <c r="B21" s="3" t="n">
+        <v>3</v>
       </c>
       <c r="C21" s="4" t="n">
         <v>44350.5927199074</v>
@@ -865,7 +832,7 @@
         <v>20</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>22</v>
@@ -876,10 +843,10 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
+      </c>
+      <c r="B22" s="3" t="n">
+        <v>3</v>
       </c>
       <c r="C22" s="4" t="n">
         <v>44350.6540625</v>
@@ -891,7 +858,7 @@
         <v>20</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>22</v>
@@ -902,10 +869,10 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
+      </c>
+      <c r="B23" s="3" t="n">
+        <v>3</v>
       </c>
       <c r="C23" s="4" t="n">
         <v>44350.7331018519</v>
@@ -917,7 +884,7 @@
         <v>20</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>22</v>
@@ -928,10 +895,10 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
+      </c>
+      <c r="B24" s="3" t="n">
+        <v>3</v>
       </c>
       <c r="C24" s="4" t="n">
         <v>44350.7532291667</v>
@@ -943,7 +910,7 @@
         <v>20</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>22</v>
@@ -953,23 +920,23 @@
       </c>
     </row>
     <row r="25" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="6" t="n">
+      <c r="A25" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="C25" s="5" t="n">
         <v>44350.7556134259</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F25" s="5" t="s">
-        <v>27</v>
+      <c r="F25" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>22</v>
@@ -980,10 +947,10 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
+      </c>
+      <c r="B26" s="3" t="n">
+        <v>3</v>
       </c>
       <c r="C26" s="4" t="n">
         <v>44351.250150463</v>
@@ -995,7 +962,7 @@
         <v>20</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>22</v>
@@ -1006,10 +973,10 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
+      </c>
+      <c r="B27" s="3" t="n">
+        <v>3</v>
       </c>
       <c r="C27" s="4" t="n">
         <v>44351.289849537</v>
@@ -1021,7 +988,7 @@
         <v>20</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>22</v>
@@ -1032,10 +999,10 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
+      </c>
+      <c r="B28" s="3" t="n">
+        <v>3</v>
       </c>
       <c r="C28" s="4" t="n">
         <v>44351.2898842593</v>
@@ -1047,7 +1014,7 @@
         <v>20</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>22</v>
@@ -1058,10 +1025,10 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
+      </c>
+      <c r="B29" s="3" t="n">
+        <v>3</v>
       </c>
       <c r="C29" s="4" t="n">
         <v>44351.4128935185</v>
@@ -1073,7 +1040,7 @@
         <v>20</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>22</v>
@@ -1084,10 +1051,10 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
+      </c>
+      <c r="B30" s="3" t="n">
+        <v>3</v>
       </c>
       <c r="C30" s="4" t="n">
         <v>44351.4252314815</v>
@@ -1099,7 +1066,7 @@
         <v>20</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>22</v>
@@ -1110,10 +1077,10 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
+      </c>
+      <c r="B31" s="3" t="n">
+        <v>3</v>
       </c>
       <c r="C31" s="4" t="n">
         <v>44351.4253240741</v>
@@ -1125,7 +1092,7 @@
         <v>20</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>22</v>
@@ -1136,10 +1103,10 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
+      </c>
+      <c r="B32" s="3" t="n">
+        <v>3</v>
       </c>
       <c r="C32" s="4" t="n">
         <v>44351.5128009259</v>
@@ -1151,7 +1118,7 @@
         <v>20</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>22</v>
@@ -1161,22 +1128,22 @@
       </c>
     </row>
     <row r="33" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" s="6" t="n">
+      <c r="A33" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C33" s="5" t="n">
         <v>44350.237037037</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F33" s="6" t="s">
         <v>25</v>
       </c>
       <c r="G33" s="3" t="s">
@@ -1187,22 +1154,22 @@
       </c>
     </row>
     <row r="34" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="6" t="n">
+      <c r="A34" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C34" s="5" t="n">
         <v>44350.7507638889</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F34" s="6" t="s">
         <v>21</v>
       </c>
       <c r="G34" s="3" t="s">
@@ -1214,10 +1181,10 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>33</v>
+        <v>18</v>
+      </c>
+      <c r="B35" s="3" t="n">
+        <v>4</v>
       </c>
       <c r="C35" s="4" t="n">
         <v>44351.5214236111</v>
@@ -1239,23 +1206,23 @@
       </c>
     </row>
     <row r="36" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" s="6" t="n">
+      <c r="A36" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C36" s="5" t="n">
         <v>44350.753287037</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F36" s="5" t="s">
-        <v>29</v>
+      <c r="F36" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>22</v>
@@ -1266,10 +1233,10 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>34</v>
+        <v>18</v>
+      </c>
+      <c r="B37" s="3" t="n">
+        <v>5</v>
       </c>
       <c r="C37" s="4" t="n">
         <v>44351.2522800926</v>
@@ -1281,7 +1248,7 @@
         <v>20</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>22</v>
@@ -1292,10 +1259,10 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>35</v>
+        <v>18</v>
+      </c>
+      <c r="B38" s="3" t="n">
+        <v>6</v>
       </c>
       <c r="C38" s="4" t="n">
         <v>44351.2455555556</v>
@@ -1307,7 +1274,7 @@
         <v>20</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>22</v>
@@ -1318,10 +1285,10 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B39" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C39" s="4" t="n">
         <v>44350.7453240741</v>
@@ -1333,7 +1300,7 @@
         <v>20</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>22</v>
@@ -1343,23 +1310,23 @@
       </c>
     </row>
     <row r="40" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C40" s="6" t="n">
+      <c r="A40" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="C40" s="5" t="n">
         <v>44350.7472453704</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F40" s="5" t="s">
-        <v>31</v>
+      <c r="F40" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>22</v>
@@ -1370,10 +1337,10 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B41" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C41" s="4" t="n">
         <v>44350.8647800926</v>
@@ -1385,7 +1352,7 @@
         <v>20</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G41" s="3" t="s">
         <v>22</v>
@@ -1396,10 +1363,10 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B42" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C42" s="4" t="n">
         <v>44350.8727430556</v>
@@ -1411,7 +1378,7 @@
         <v>20</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>22</v>
@@ -1422,10 +1389,10 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B43" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C43" s="4" t="n">
         <v>44350.8742592593</v>
@@ -1437,7 +1404,7 @@
         <v>20</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>22</v>
@@ -1448,10 +1415,10 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B44" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C44" s="4" t="n">
         <v>44350.8748726852</v>
@@ -1463,7 +1430,7 @@
         <v>20</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>22</v>
@@ -1474,10 +1441,10 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B45" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C45" s="4" t="n">
         <v>44350.8758912037</v>
@@ -1489,7 +1456,7 @@
         <v>20</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>22</v>
@@ -1500,10 +1467,10 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B46" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C46" s="4" t="n">
         <v>44350.8775462963</v>
@@ -1515,7 +1482,7 @@
         <v>20</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>22</v>
@@ -1526,10 +1493,10 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B47" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C47" s="4" t="n">
         <v>44350.8818402778</v>
@@ -1541,7 +1508,7 @@
         <v>20</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>22</v>
@@ -1552,10 +1519,10 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B48" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C48" s="4" t="n">
         <v>44350.8848148148</v>
@@ -1567,7 +1534,7 @@
         <v>20</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>22</v>
@@ -1578,10 +1545,10 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B49" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C49" s="4" t="n">
         <v>44350.9454513889</v>
@@ -1593,7 +1560,7 @@
         <v>20</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>22</v>
@@ -1604,10 +1571,10 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B50" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C50" s="4" t="n">
         <v>44350.9466898148</v>
@@ -1619,7 +1586,7 @@
         <v>20</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>22</v>
@@ -1630,10 +1597,10 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B51" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C51" s="4" t="n">
         <v>44350.9478935185</v>
@@ -1645,7 +1612,7 @@
         <v>20</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>22</v>
@@ -1656,10 +1623,10 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B52" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C52" s="4" t="n">
         <v>44350.950787037</v>
@@ -1671,7 +1638,7 @@
         <v>20</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>22</v>
@@ -1682,10 +1649,10 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B53" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C53" s="4" t="n">
         <v>44350.9559143518</v>
@@ -1697,7 +1664,7 @@
         <v>20</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>22</v>
@@ -1708,10 +1675,10 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B54" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C54" s="4" t="n">
         <v>44351.0078125</v>
@@ -1723,7 +1690,7 @@
         <v>20</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>22</v>
@@ -1734,10 +1701,10 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B55" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C55" s="4" t="n">
         <v>44351.1466087963</v>
@@ -1749,7 +1716,7 @@
         <v>20</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>22</v>
@@ -1760,10 +1727,10 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B56" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C56" s="4" t="n">
         <v>44351.1521296296</v>
@@ -1775,7 +1742,7 @@
         <v>20</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>22</v>
@@ -1786,10 +1753,10 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B57" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C57" s="4" t="n">
         <v>44351.1742476852</v>
@@ -1801,7 +1768,7 @@
         <v>20</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>22</v>
@@ -1812,10 +1779,10 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B58" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C58" s="4" t="n">
         <v>44351.1795949074</v>
@@ -1827,7 +1794,7 @@
         <v>20</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>22</v>
@@ -1838,10 +1805,10 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B59" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C59" s="4" t="n">
         <v>44351.1801851852</v>
@@ -1853,7 +1820,7 @@
         <v>20</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G59" s="3" t="s">
         <v>22</v>
@@ -1864,10 +1831,10 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B60" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C60" s="4" t="n">
         <v>44351.1809143519</v>
@@ -1879,7 +1846,7 @@
         <v>20</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>22</v>
@@ -1890,10 +1857,10 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B61" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C61" s="4" t="n">
         <v>44351.1830208333</v>
@@ -1905,7 +1872,7 @@
         <v>20</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G61" s="3" t="s">
         <v>22</v>
@@ -1916,10 +1883,10 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B62" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C62" s="4" t="n">
         <v>44351.1832291667</v>
@@ -1931,7 +1898,7 @@
         <v>20</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G62" s="3" t="s">
         <v>22</v>
@@ -1942,10 +1909,10 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B63" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C63" s="4" t="n">
         <v>44351.1864236111</v>
@@ -1957,7 +1924,7 @@
         <v>20</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G63" s="3" t="s">
         <v>22</v>
@@ -1968,10 +1935,10 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B64" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C64" s="4" t="n">
         <v>44351.1871296296</v>
@@ -1983,7 +1950,7 @@
         <v>20</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G64" s="3" t="s">
         <v>22</v>
@@ -1994,10 +1961,10 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B65" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C65" s="4" t="n">
         <v>44351.1899305556</v>
@@ -2009,7 +1976,7 @@
         <v>20</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G65" s="3" t="s">
         <v>22</v>
@@ -2020,10 +1987,10 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B66" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C66" s="4" t="n">
         <v>44351.192037037</v>
@@ -2035,7 +2002,7 @@
         <v>20</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G66" s="3" t="s">
         <v>22</v>
@@ -2046,10 +2013,10 @@
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B67" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C67" s="4" t="n">
         <v>44351.1936111111</v>
@@ -2061,7 +2028,7 @@
         <v>20</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G67" s="3" t="s">
         <v>22</v>
@@ -2072,10 +2039,10 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B68" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C68" s="4" t="n">
         <v>44351.229212963</v>
@@ -2087,7 +2054,7 @@
         <v>20</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G68" s="3" t="s">
         <v>22</v>
@@ -2098,10 +2065,10 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B69" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C69" s="4" t="n">
         <v>44351.2294560185</v>
@@ -2113,7 +2080,7 @@
         <v>20</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G69" s="3" t="s">
         <v>22</v>
@@ -2124,10 +2091,10 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="B70" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="C70" s="4" t="n">
         <v>44351.2303125</v>
@@ -2139,7 +2106,7 @@
         <v>20</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G70" s="3" t="s">
         <v>22</v>
@@ -2149,23 +2116,23 @@
       </c>
     </row>
     <row r="71" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C71" s="6" t="n">
+      <c r="A71" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B71" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="C71" s="5" t="n">
         <v>44351.2468518519</v>
       </c>
-      <c r="D71" s="5" t="s">
+      <c r="D71" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F71" s="5" t="s">
-        <v>27</v>
+      <c r="F71" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="G71" s="3" t="s">
         <v>22</v>
@@ -2176,10 +2143,10 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B72" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C72" s="4" t="n">
         <v>44350.2428472222</v>
@@ -2191,7 +2158,7 @@
         <v>20</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G72" s="3" t="s">
         <v>22</v>
@@ -2202,10 +2169,10 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B73" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C73" s="4" t="n">
         <v>44350.2429166667</v>
@@ -2217,7 +2184,7 @@
         <v>20</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G73" s="3" t="s">
         <v>22</v>
@@ -2227,23 +2194,23 @@
       </c>
     </row>
     <row r="74" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C74" s="6" t="n">
+      <c r="A74" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B74" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="C74" s="5" t="n">
         <v>44350.246400463</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="D74" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F74" s="5" t="s">
-        <v>31</v>
+      <c r="F74" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="G74" s="3" t="s">
         <v>22</v>
@@ -2254,10 +2221,10 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B75" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C75" s="4" t="n">
         <v>44350.2604398148</v>
@@ -2269,7 +2236,7 @@
         <v>20</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G75" s="3" t="s">
         <v>22</v>
@@ -2280,10 +2247,10 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B76" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C76" s="4" t="n">
         <v>44350.2627314815</v>
@@ -2295,7 +2262,7 @@
         <v>20</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G76" s="3" t="s">
         <v>22</v>
@@ -2306,10 +2273,10 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B77" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C77" s="4" t="n">
         <v>44350.353900463</v>
@@ -2321,7 +2288,7 @@
         <v>20</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G77" s="3" t="s">
         <v>22</v>
@@ -2332,10 +2299,10 @@
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B78" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C78" s="4" t="n">
         <v>44350.3546296296</v>
@@ -2347,7 +2314,7 @@
         <v>20</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G78" s="3" t="s">
         <v>22</v>
@@ -2358,10 +2325,10 @@
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B79" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C79" s="4" t="n">
         <v>44350.3572106482</v>
@@ -2373,7 +2340,7 @@
         <v>20</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G79" s="3" t="s">
         <v>22</v>
@@ -2384,10 +2351,10 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B80" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C80" s="4" t="n">
         <v>44350.3879861111</v>
@@ -2399,7 +2366,7 @@
         <v>20</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G80" s="3" t="s">
         <v>22</v>
@@ -2410,10 +2377,10 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B81" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C81" s="4" t="n">
         <v>44350.3886342593</v>
@@ -2425,7 +2392,7 @@
         <v>20</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G81" s="3" t="s">
         <v>22</v>
@@ -2436,10 +2403,10 @@
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B82" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C82" s="4" t="n">
         <v>44350.449375</v>
@@ -2451,7 +2418,7 @@
         <v>20</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G82" s="3" t="s">
         <v>22</v>
@@ -2462,10 +2429,10 @@
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B83" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C83" s="4" t="n">
         <v>44350.4525347222</v>
@@ -2477,7 +2444,7 @@
         <v>20</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G83" s="3" t="s">
         <v>22</v>
@@ -2488,10 +2455,10 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B84" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C84" s="4" t="n">
         <v>44350.4670717593</v>
@@ -2503,7 +2470,7 @@
         <v>20</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G84" s="3" t="s">
         <v>22</v>
@@ -2514,10 +2481,10 @@
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B85" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C85" s="4" t="n">
         <v>44350.4743518519</v>
@@ -2529,7 +2496,7 @@
         <v>20</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G85" s="3" t="s">
         <v>22</v>
@@ -2540,10 +2507,10 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B86" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C86" s="4" t="n">
         <v>44350.5694907407</v>
@@ -2555,7 +2522,7 @@
         <v>20</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G86" s="3" t="s">
         <v>22</v>
@@ -2566,10 +2533,10 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B87" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C87" s="4" t="n">
         <v>44350.5695833333</v>
@@ -2581,7 +2548,7 @@
         <v>20</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G87" s="3" t="s">
         <v>22</v>
@@ -2592,10 +2559,10 @@
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B88" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C88" s="4" t="n">
         <v>44350.5732986111</v>
@@ -2607,7 +2574,7 @@
         <v>20</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G88" s="3" t="s">
         <v>22</v>
@@ -2618,10 +2585,10 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B89" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C89" s="4" t="n">
         <v>44350.5733449074</v>
@@ -2633,7 +2600,7 @@
         <v>20</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G89" s="3" t="s">
         <v>22</v>
@@ -2644,10 +2611,10 @@
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B90" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C90" s="4" t="n">
         <v>44350.6504513889</v>
@@ -2659,7 +2626,7 @@
         <v>20</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G90" s="3" t="s">
         <v>22</v>
@@ -2670,10 +2637,10 @@
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B91" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C91" s="4" t="n">
         <v>44350.6564351852</v>
@@ -2685,7 +2652,7 @@
         <v>20</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G91" s="3" t="s">
         <v>22</v>
@@ -2696,10 +2663,10 @@
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B92" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C92" s="4" t="n">
         <v>44350.7102546296</v>
@@ -2711,7 +2678,7 @@
         <v>20</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G92" s="3" t="s">
         <v>22</v>
@@ -2722,10 +2689,10 @@
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B93" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C93" s="4" t="n">
         <v>44350.7103240741</v>
@@ -2737,7 +2704,7 @@
         <v>20</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G93" s="3" t="s">
         <v>22</v>
@@ -2748,10 +2715,10 @@
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B94" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C94" s="4" t="n">
         <v>44350.7149537037</v>
@@ -2763,7 +2730,7 @@
         <v>20</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G94" s="3" t="s">
         <v>22</v>
@@ -2773,23 +2740,23 @@
       </c>
     </row>
     <row r="95" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C95" s="6" t="n">
+      <c r="A95" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B95" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="C95" s="5" t="n">
         <v>44350.7470949074</v>
       </c>
-      <c r="D95" s="5" t="s">
+      <c r="D95" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F95" s="5" t="s">
-        <v>27</v>
+      <c r="F95" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="G95" s="3" t="s">
         <v>22</v>
@@ -2800,10 +2767,10 @@
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B96" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C96" s="4" t="n">
         <v>44351.2456597222</v>
@@ -2815,7 +2782,7 @@
         <v>20</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G96" s="3" t="s">
         <v>22</v>
@@ -2826,10 +2793,10 @@
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B97" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C97" s="4" t="n">
         <v>44351.259837963</v>
@@ -2841,7 +2808,7 @@
         <v>20</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G97" s="3" t="s">
         <v>22</v>
@@ -2852,10 +2819,10 @@
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B98" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C98" s="4" t="n">
         <v>44351.2627314815</v>
@@ -2867,7 +2834,7 @@
         <v>20</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G98" s="3" t="s">
         <v>22</v>
@@ -2878,10 +2845,10 @@
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B99" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C99" s="4" t="n">
         <v>44351.4434722222</v>
@@ -2893,7 +2860,7 @@
         <v>20</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G99" s="3" t="s">
         <v>22</v>
@@ -2904,10 +2871,10 @@
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B100" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C100" s="4" t="n">
         <v>44351.4464351852</v>
@@ -2919,7 +2886,7 @@
         <v>20</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G100" s="3" t="s">
         <v>22</v>
@@ -2930,10 +2897,10 @@
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B101" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C101" s="4" t="n">
         <v>44351.4585532407</v>
@@ -2945,7 +2912,7 @@
         <v>20</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G101" s="3" t="s">
         <v>22</v>
@@ -2956,10 +2923,10 @@
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B102" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C102" s="4" t="n">
         <v>44351.4645833333</v>
@@ -2971,7 +2938,7 @@
         <v>20</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G102" s="3" t="s">
         <v>22</v>
@@ -2982,10 +2949,10 @@
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B103" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C103" s="4" t="n">
         <v>44351.522037037</v>
@@ -2997,7 +2964,7 @@
         <v>20</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G103" s="3" t="s">
         <v>22</v>
@@ -3008,10 +2975,10 @@
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B104" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="C104" s="4" t="n">
         <v>44351.5248958333</v>
@@ -3023,7 +2990,7 @@
         <v>20</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G104" s="3" t="s">
         <v>22</v>
@@ -3034,10 +3001,10 @@
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>54</v>
+        <v>18</v>
+      </c>
+      <c r="B105" s="3" t="n">
+        <v>9</v>
       </c>
       <c r="C105" s="4" t="n">
         <v>44350.2324537037</v>
@@ -3049,7 +3016,7 @@
         <v>20</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G105" s="3" t="s">
         <v>22</v>
@@ -3060,10 +3027,10 @@
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B106" s="3" t="s">
-        <v>54</v>
+        <v>18</v>
+      </c>
+      <c r="B106" s="3" t="n">
+        <v>9</v>
       </c>
       <c r="C106" s="4" t="n">
         <v>44350.2328935185</v>
@@ -3075,7 +3042,7 @@
         <v>20</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G106" s="3" t="s">
         <v>22</v>
@@ -3086,10 +3053,10 @@
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>54</v>
+        <v>18</v>
+      </c>
+      <c r="B107" s="3" t="n">
+        <v>9</v>
       </c>
       <c r="C107" s="4" t="n">
         <v>44350.2335300926</v>
@@ -3101,7 +3068,7 @@
         <v>20</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G107" s="3" t="s">
         <v>22</v>
@@ -3112,10 +3079,10 @@
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>54</v>
+        <v>18</v>
+      </c>
+      <c r="B108" s="3" t="n">
+        <v>9</v>
       </c>
       <c r="C108" s="4" t="n">
         <v>44350.2337847222</v>
@@ -3127,7 +3094,7 @@
         <v>20</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G108" s="3" t="s">
         <v>22</v>
@@ -3138,10 +3105,10 @@
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>54</v>
+        <v>18</v>
+      </c>
+      <c r="B109" s="3" t="n">
+        <v>9</v>
       </c>
       <c r="C109" s="4" t="n">
         <v>44350.2342939815</v>
@@ -3153,7 +3120,7 @@
         <v>20</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G109" s="3" t="s">
         <v>22</v>
@@ -3164,10 +3131,10 @@
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B110" s="3" t="s">
-        <v>54</v>
+        <v>18</v>
+      </c>
+      <c r="B110" s="3" t="n">
+        <v>9</v>
       </c>
       <c r="C110" s="4" t="n">
         <v>44350.2343518519</v>
@@ -3179,7 +3146,7 @@
         <v>20</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G110" s="3" t="s">
         <v>22</v>
@@ -3190,10 +3157,10 @@
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>54</v>
+        <v>18</v>
+      </c>
+      <c r="B111" s="3" t="n">
+        <v>9</v>
       </c>
       <c r="C111" s="4" t="n">
         <v>44350.2473958333</v>
@@ -3205,7 +3172,7 @@
         <v>20</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G111" s="3" t="s">
         <v>22</v>
@@ -3216,10 +3183,10 @@
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B112" s="3" t="s">
-        <v>55</v>
+        <v>18</v>
+      </c>
+      <c r="B112" s="3" t="n">
+        <v>10</v>
       </c>
       <c r="C112" s="4" t="n">
         <v>44350.2516319444</v>
@@ -3231,7 +3198,7 @@
         <v>20</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="G112" s="3" t="s">
         <v>22</v>
@@ -3242,10 +3209,10 @@
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>55</v>
+        <v>18</v>
+      </c>
+      <c r="B113" s="3" t="n">
+        <v>10</v>
       </c>
       <c r="C113" s="4" t="n">
         <v>44350.257025463</v>
@@ -3257,7 +3224,7 @@
         <v>20</v>
       </c>
       <c r="F113" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G113" s="3" t="s">
         <v>22</v>
@@ -3268,10 +3235,10 @@
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>55</v>
+        <v>18</v>
+      </c>
+      <c r="B114" s="3" t="n">
+        <v>10</v>
       </c>
       <c r="C114" s="4" t="n">
         <v>44350.7423842593</v>
@@ -3283,7 +3250,7 @@
         <v>20</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G114" s="3" t="s">
         <v>22</v>
@@ -3293,23 +3260,23 @@
       </c>
     </row>
     <row r="115" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B115" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C115" s="6" t="n">
+      <c r="A115" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B115" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="C115" s="5" t="n">
         <v>44350.7499652778</v>
       </c>
-      <c r="D115" s="5" t="s">
+      <c r="D115" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F115" s="5" t="s">
-        <v>36</v>
+      <c r="F115" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="G115" s="3" t="s">
         <v>22</v>
@@ -3319,23 +3286,23 @@
       </c>
     </row>
     <row r="116" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B116" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C116" s="6" t="n">
+      <c r="A116" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B116" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="C116" s="5" t="n">
         <v>44351.2462615741</v>
       </c>
-      <c r="D116" s="5" t="s">
+      <c r="D116" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F116" s="5" t="s">
-        <v>56</v>
+      <c r="F116" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="G116" s="3" t="s">
         <v>22</v>
@@ -3346,10 +3313,10 @@
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B117" s="3" t="s">
-        <v>55</v>
+        <v>18</v>
+      </c>
+      <c r="B117" s="3" t="n">
+        <v>10</v>
       </c>
       <c r="C117" s="4" t="n">
         <v>44351.2519791667</v>
@@ -3361,7 +3328,7 @@
         <v>20</v>
       </c>
       <c r="F117" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G117" s="3" t="s">
         <v>22</v>
@@ -3372,10 +3339,10 @@
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B118" s="3" t="s">
-        <v>57</v>
+        <v>18</v>
+      </c>
+      <c r="B118" s="3" t="n">
+        <v>11</v>
       </c>
       <c r="C118" s="4" t="n">
         <v>44350.244849537</v>
@@ -3387,7 +3354,7 @@
         <v>20</v>
       </c>
       <c r="F118" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G118" s="3" t="s">
         <v>22</v>
@@ -3397,23 +3364,23 @@
       </c>
     </row>
     <row r="119" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B119" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C119" s="6" t="n">
+      <c r="A119" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B119" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="C119" s="5" t="n">
         <v>44350.2511226852</v>
       </c>
-      <c r="D119" s="5" t="s">
+      <c r="D119" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F119" s="5" t="s">
-        <v>36</v>
+      <c r="F119" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="G119" s="3" t="s">
         <v>22</v>
@@ -3423,23 +3390,23 @@
       </c>
     </row>
     <row r="120" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B120" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C120" s="6" t="n">
+      <c r="A120" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B120" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="C120" s="5" t="n">
         <v>44350.7510763889</v>
       </c>
-      <c r="D120" s="5" t="s">
+      <c r="D120" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F120" s="5" t="s">
-        <v>56</v>
+      <c r="F120" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="G120" s="3" t="s">
         <v>22</v>
@@ -3450,10 +3417,10 @@
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>57</v>
+        <v>18</v>
+      </c>
+      <c r="B121" s="3" t="n">
+        <v>11</v>
       </c>
       <c r="C121" s="4" t="n">
         <v>44350.7565972222</v>
@@ -3465,7 +3432,7 @@
         <v>20</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G121" s="3" t="s">
         <v>22</v>
@@ -3475,23 +3442,23 @@
       </c>
     </row>
     <row r="122" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B122" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C122" s="6" t="n">
+      <c r="A122" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B122" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="C122" s="5" t="n">
         <v>44350.2824421296</v>
       </c>
-      <c r="D122" s="5" t="s">
+      <c r="D122" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F122" s="5" t="s">
-        <v>41</v>
+      <c r="F122" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="G122" s="3" t="s">
         <v>22</v>
@@ -3502,10 +3469,10 @@
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B123" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B123" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C123" s="4" t="n">
         <v>44350.2826967593</v>
@@ -3517,7 +3484,7 @@
         <v>20</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G123" s="3" t="s">
         <v>22</v>
@@ -3528,10 +3495,10 @@
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B124" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B124" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C124" s="4" t="n">
         <v>44350.2853356482</v>
@@ -3543,7 +3510,7 @@
         <v>20</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G124" s="3" t="s">
         <v>22</v>
@@ -3554,10 +3521,10 @@
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B125" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C125" s="4" t="n">
         <v>44350.2880208333</v>
@@ -3569,7 +3536,7 @@
         <v>20</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="G125" s="3" t="s">
         <v>22</v>
@@ -3580,10 +3547,10 @@
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B126" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C126" s="4" t="n">
         <v>44350.2894212963</v>
@@ -3595,7 +3562,7 @@
         <v>20</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G126" s="3" t="s">
         <v>22</v>
@@ -3606,10 +3573,10 @@
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B127" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C127" s="4" t="n">
         <v>44350.2918981481</v>
@@ -3621,7 +3588,7 @@
         <v>20</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G127" s="3" t="s">
         <v>22</v>
@@ -3632,10 +3599,10 @@
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B128" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B128" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C128" s="4" t="n">
         <v>44350.294525463</v>
@@ -3647,7 +3614,7 @@
         <v>20</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G128" s="3" t="s">
         <v>22</v>
@@ -3658,10 +3625,10 @@
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B129" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B129" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C129" s="4" t="n">
         <v>44350.324224537</v>
@@ -3673,7 +3640,7 @@
         <v>20</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G129" s="3" t="s">
         <v>22</v>
@@ -3684,10 +3651,10 @@
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B130" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B130" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C130" s="4" t="n">
         <v>44350.3244444444</v>
@@ -3699,7 +3666,7 @@
         <v>20</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G130" s="3" t="s">
         <v>22</v>
@@ -3710,10 +3677,10 @@
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B131" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B131" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C131" s="4" t="n">
         <v>44350.3328935185</v>
@@ -3725,7 +3692,7 @@
         <v>20</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G131" s="3" t="s">
         <v>22</v>
@@ -3736,10 +3703,10 @@
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B132" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C132" s="4" t="n">
         <v>44350.3330092593</v>
@@ -3751,7 +3718,7 @@
         <v>20</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G132" s="3" t="s">
         <v>22</v>
@@ -3762,10 +3729,10 @@
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B133" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B133" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C133" s="4" t="n">
         <v>44350.3338541667</v>
@@ -3777,7 +3744,7 @@
         <v>20</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G133" s="3" t="s">
         <v>22</v>
@@ -3788,10 +3755,10 @@
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B134" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B134" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C134" s="4" t="n">
         <v>44350.334375</v>
@@ -3803,7 +3770,7 @@
         <v>20</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G134" s="3" t="s">
         <v>22</v>
@@ -3814,10 +3781,10 @@
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B135" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B135" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C135" s="4" t="n">
         <v>44350.3487152778</v>
@@ -3829,7 +3796,7 @@
         <v>20</v>
       </c>
       <c r="F135" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G135" s="3" t="s">
         <v>22</v>
@@ -3840,10 +3807,10 @@
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B136" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B136" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C136" s="4" t="n">
         <v>44350.3686111111</v>
@@ -3855,7 +3822,7 @@
         <v>20</v>
       </c>
       <c r="F136" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G136" s="3" t="s">
         <v>22</v>
@@ -3866,10 +3833,10 @@
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B137" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B137" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C137" s="4" t="n">
         <v>44350.4617476852</v>
@@ -3881,7 +3848,7 @@
         <v>20</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G137" s="3" t="s">
         <v>22</v>
@@ -3892,10 +3859,10 @@
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B138" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B138" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C138" s="4" t="n">
         <v>44350.461875</v>
@@ -3907,7 +3874,7 @@
         <v>20</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G138" s="3" t="s">
         <v>22</v>
@@ -3918,10 +3885,10 @@
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B139" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B139" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C139" s="4" t="n">
         <v>44350.5475231481</v>
@@ -3933,7 +3900,7 @@
         <v>20</v>
       </c>
       <c r="F139" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G139" s="3" t="s">
         <v>22</v>
@@ -3944,10 +3911,10 @@
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B140" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B140" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C140" s="4" t="n">
         <v>44350.5476967593</v>
@@ -3959,7 +3926,7 @@
         <v>20</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G140" s="3" t="s">
         <v>22</v>
@@ -3970,10 +3937,10 @@
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B141" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B141" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C141" s="4" t="n">
         <v>44350.5763078704</v>
@@ -3985,7 +3952,7 @@
         <v>20</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G141" s="3" t="s">
         <v>22</v>
@@ -3996,10 +3963,10 @@
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B142" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B142" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C142" s="4" t="n">
         <v>44350.5765046296</v>
@@ -4011,7 +3978,7 @@
         <v>20</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G142" s="3" t="s">
         <v>22</v>
@@ -4022,10 +3989,10 @@
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B143" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C143" s="4" t="n">
         <v>44350.5779166667</v>
@@ -4037,7 +4004,7 @@
         <v>20</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G143" s="3" t="s">
         <v>22</v>
@@ -4048,10 +4015,10 @@
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B144" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B144" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C144" s="4" t="n">
         <v>44350.5919907407</v>
@@ -4063,7 +4030,7 @@
         <v>20</v>
       </c>
       <c r="F144" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G144" s="3" t="s">
         <v>22</v>
@@ -4074,10 +4041,10 @@
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B145" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B145" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C145" s="4" t="n">
         <v>44350.5922337963</v>
@@ -4089,7 +4056,7 @@
         <v>20</v>
       </c>
       <c r="F145" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G145" s="3" t="s">
         <v>22</v>
@@ -4100,10 +4067,10 @@
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B146" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B146" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C146" s="4" t="n">
         <v>44350.5971064815</v>
@@ -4115,7 +4082,7 @@
         <v>20</v>
       </c>
       <c r="F146" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G146" s="3" t="s">
         <v>22</v>
@@ -4126,10 +4093,10 @@
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B147" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B147" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C147" s="4" t="n">
         <v>44350.6431134259</v>
@@ -4141,7 +4108,7 @@
         <v>20</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G147" s="3" t="s">
         <v>22</v>
@@ -4152,10 +4119,10 @@
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B148" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B148" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C148" s="4" t="n">
         <v>44350.6436689815</v>
@@ -4167,7 +4134,7 @@
         <v>20</v>
       </c>
       <c r="F148" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G148" s="3" t="s">
         <v>22</v>
@@ -4178,10 +4145,10 @@
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B149" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B149" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C149" s="4" t="n">
         <v>44350.662974537</v>
@@ -4193,7 +4160,7 @@
         <v>20</v>
       </c>
       <c r="F149" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G149" s="3" t="s">
         <v>22</v>
@@ -4204,10 +4171,10 @@
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B150" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B150" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C150" s="4" t="n">
         <v>44350.6631597222</v>
@@ -4219,7 +4186,7 @@
         <v>20</v>
       </c>
       <c r="F150" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G150" s="3" t="s">
         <v>22</v>
@@ -4230,10 +4197,10 @@
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B151" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B151" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C151" s="4" t="n">
         <v>44350.6786111111</v>
@@ -4245,7 +4212,7 @@
         <v>20</v>
       </c>
       <c r="F151" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G151" s="3" t="s">
         <v>22</v>
@@ -4256,10 +4223,10 @@
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B152" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B152" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C152" s="4" t="n">
         <v>44350.681087963</v>
@@ -4271,7 +4238,7 @@
         <v>20</v>
       </c>
       <c r="F152" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G152" s="3" t="s">
         <v>22</v>
@@ -4282,10 +4249,10 @@
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B153" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B153" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C153" s="4" t="n">
         <v>44350.7084606482</v>
@@ -4297,7 +4264,7 @@
         <v>20</v>
       </c>
       <c r="F153" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G153" s="3" t="s">
         <v>22</v>
@@ -4308,10 +4275,10 @@
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B154" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B154" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C154" s="4" t="n">
         <v>44350.7085763889</v>
@@ -4323,7 +4290,7 @@
         <v>20</v>
       </c>
       <c r="F154" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G154" s="3" t="s">
         <v>22</v>
@@ -4334,10 +4301,10 @@
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B155" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B155" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C155" s="4" t="n">
         <v>44350.7096875</v>
@@ -4349,7 +4316,7 @@
         <v>20</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G155" s="3" t="s">
         <v>22</v>
@@ -4360,10 +4327,10 @@
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B156" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B156" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C156" s="4" t="n">
         <v>44350.7129861111</v>
@@ -4375,7 +4342,7 @@
         <v>20</v>
       </c>
       <c r="F156" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G156" s="3" t="s">
         <v>22</v>
@@ -4386,10 +4353,10 @@
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B157" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B157" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C157" s="4" t="n">
         <v>44350.7195949074</v>
@@ -4401,7 +4368,7 @@
         <v>20</v>
       </c>
       <c r="F157" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G157" s="3" t="s">
         <v>22</v>
@@ -4412,10 +4379,10 @@
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B158" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B158" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C158" s="4" t="n">
         <v>44350.7197916667</v>
@@ -4427,7 +4394,7 @@
         <v>20</v>
       </c>
       <c r="F158" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G158" s="3" t="s">
         <v>22</v>
@@ -4438,10 +4405,10 @@
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B159" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B159" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C159" s="4" t="n">
         <v>44350.7237847222</v>
@@ -4453,7 +4420,7 @@
         <v>20</v>
       </c>
       <c r="F159" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G159" s="3" t="s">
         <v>22</v>
@@ -4464,10 +4431,10 @@
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B160" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B160" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C160" s="4" t="n">
         <v>44350.7239814815</v>
@@ -4479,7 +4446,7 @@
         <v>20</v>
       </c>
       <c r="F160" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G160" s="3" t="s">
         <v>22</v>
@@ -4490,10 +4457,10 @@
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B161" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B161" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C161" s="4" t="n">
         <v>44350.7290856481</v>
@@ -4505,7 +4472,7 @@
         <v>20</v>
       </c>
       <c r="F161" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G161" s="3" t="s">
         <v>22</v>
@@ -4515,23 +4482,23 @@
       </c>
     </row>
     <row r="162" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B162" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C162" s="6" t="n">
+      <c r="A162" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B162" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="C162" s="5" t="n">
         <v>44350.7293402778</v>
       </c>
-      <c r="D162" s="5" t="s">
+      <c r="D162" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F162" s="5" t="s">
-        <v>40</v>
+      <c r="F162" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="G162" s="3" t="s">
         <v>22</v>
@@ -4542,10 +4509,10 @@
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B163" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B163" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C163" s="4" t="n">
         <v>44351.2884490741</v>
@@ -4557,7 +4524,7 @@
         <v>20</v>
       </c>
       <c r="F163" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G163" s="3" t="s">
         <v>22</v>
@@ -4568,10 +4535,10 @@
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B164" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B164" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C164" s="4" t="n">
         <v>44351.2886689815</v>
@@ -4583,7 +4550,7 @@
         <v>20</v>
       </c>
       <c r="F164" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G164" s="3" t="s">
         <v>22</v>
@@ -4594,10 +4561,10 @@
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B165" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B165" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C165" s="4" t="n">
         <v>44351.2906134259</v>
@@ -4609,7 +4576,7 @@
         <v>20</v>
       </c>
       <c r="F165" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G165" s="3" t="s">
         <v>22</v>
@@ -4620,10 +4587,10 @@
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B166" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B166" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C166" s="4" t="n">
         <v>44351.2926388889</v>
@@ -4635,7 +4602,7 @@
         <v>20</v>
       </c>
       <c r="F166" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="G166" s="3" t="s">
         <v>22</v>
@@ -4646,10 +4613,10 @@
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B167" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B167" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C167" s="4" t="n">
         <v>44351.2941319444</v>
@@ -4661,7 +4628,7 @@
         <v>20</v>
       </c>
       <c r="F167" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G167" s="3" t="s">
         <v>22</v>
@@ -4672,10 +4639,10 @@
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B168" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B168" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C168" s="4" t="n">
         <v>44351.2961458333</v>
@@ -4687,7 +4654,7 @@
         <v>20</v>
       </c>
       <c r="F168" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G168" s="3" t="s">
         <v>22</v>
@@ -4698,10 +4665,10 @@
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B169" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B169" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C169" s="4" t="n">
         <v>44351.2983101852</v>
@@ -4713,7 +4680,7 @@
         <v>20</v>
       </c>
       <c r="F169" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G169" s="3" t="s">
         <v>22</v>
@@ -4724,10 +4691,10 @@
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B170" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B170" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C170" s="4" t="n">
         <v>44351.3538541667</v>
@@ -4739,7 +4706,7 @@
         <v>20</v>
       </c>
       <c r="F170" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G170" s="3" t="s">
         <v>22</v>
@@ -4750,10 +4717,10 @@
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B171" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B171" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C171" s="4" t="n">
         <v>44351.3734606481</v>
@@ -4765,7 +4732,7 @@
         <v>20</v>
       </c>
       <c r="F171" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G171" s="3" t="s">
         <v>22</v>
@@ -4776,10 +4743,10 @@
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B172" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B172" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C172" s="4" t="n">
         <v>44351.3737152778</v>
@@ -4791,7 +4758,7 @@
         <v>20</v>
       </c>
       <c r="F172" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G172" s="3" t="s">
         <v>22</v>
@@ -4802,10 +4769,10 @@
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B173" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B173" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C173" s="4" t="n">
         <v>44351.379224537</v>
@@ -4817,7 +4784,7 @@
         <v>20</v>
       </c>
       <c r="F173" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G173" s="3" t="s">
         <v>22</v>
@@ -4828,10 +4795,10 @@
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B174" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B174" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C174" s="4" t="n">
         <v>44351.4139814815</v>
@@ -4843,7 +4810,7 @@
         <v>20</v>
       </c>
       <c r="F174" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G174" s="3" t="s">
         <v>22</v>
@@ -4854,10 +4821,10 @@
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B175" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B175" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C175" s="4" t="n">
         <v>44351.4162037037</v>
@@ -4869,7 +4836,7 @@
         <v>20</v>
       </c>
       <c r="F175" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G175" s="3" t="s">
         <v>22</v>
@@ -4880,10 +4847,10 @@
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B176" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B176" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C176" s="4" t="n">
         <v>44351.425625</v>
@@ -4895,7 +4862,7 @@
         <v>20</v>
       </c>
       <c r="F176" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G176" s="3" t="s">
         <v>22</v>
@@ -4906,10 +4873,10 @@
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B177" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B177" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="C177" s="4" t="n">
         <v>44351.4258449074</v>
@@ -4921,7 +4888,7 @@
         <v>20</v>
       </c>
       <c r="F177" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G177" s="3" t="s">
         <v>22</v>

</xml_diff>